<commit_message>
FUNCTIONALITY: Removed outdated test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/RLH Cases/LDAP/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/RLH Cases/LDAP/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -45,30 +45,12 @@
     <t>FieldMapping</t>
   </si>
   <si>
-    <t>LDAP</t>
-  </si>
-  <si>
     <t>LDAPConfiguration</t>
   </si>
   <si>
-    <t>LDAPLoadsManagerFields</t>
-  </si>
-  <si>
-    <t>All LDAP</t>
-  </si>
-  <si>
     <t>ManuallyLoadCustodians</t>
   </si>
   <si>
-    <t>OverwriteFieldsOnImport</t>
-  </si>
-  <si>
-    <t>ScheduledLDAPUpdates</t>
-  </si>
-  <si>
-    <t>Time Machine &amp; LDAP</t>
-  </si>
-  <si>
     <t>Total Tests Tracked:</t>
   </si>
   <si>
@@ -76,6 +58,12 @@
   </si>
   <si>
     <t>Percentage Automated:</t>
+  </si>
+  <si>
+    <t>Outdated, but applicable</t>
+  </si>
+  <si>
+    <t>Not yet re-implemented</t>
   </si>
 </sst>
 </file>
@@ -142,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,7 +145,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,15 +548,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.28515625" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="50.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" style="3" customWidth="1"/>
@@ -581,24 +568,24 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$2:A49)</f>
-        <v>6</v>
+        <f>COUNTA(A:A)-1</f>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7">
-        <f>COUNTIF($D$2:D49,"Ready to Write")+COUNTIF($D$2:D49,"Outdated")</f>
+      <c r="G1" s="6">
+        <f>COUNTIF(D:D,"Ready to Write")+COUNTIF(D:D,"Outdated")</f>
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -617,127 +604,81 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7">
-        <f>COUNTIF($D$2:D49,"Automated")+COUNTIF($D$2:D49,"Finished")</f>
+      <c r="G2" s="6">
+        <f>COUNTIF(D:D,"Automated")+COUNTIF(D:D,"Finished")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G4" s="3">
-        <f>SUM($C$2:C49)</f>
-        <v>55</v>
+        <f>SUM(C:C)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$2:B49)</f>
+        <f>SUM(B:B)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="10">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9">
         <f>G5/G4</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -755,7 +696,7 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="containsText" dxfId="8" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>

</xml_diff>